<commit_message>
Add metrics and configuration files for CMAEStrategy in Drop-Wave and Levi experiments
- Created metrics.csv for Drop-Wave experiment with success rate, average best fitness, best solution found, and execution time.
- Added config.json for Levi experiment specifying generation count, chromosome length, population size, bounds, fitness function, optimization method, number of executions, optimal solution, and tolerance.
- Introduced curves.xlsx for Levi experiment containing detailed execution data.
- Generated metrics.csv for Levi experiment with success rate, average best fitness, best solution found, and execution time.
</commit_message>
<xml_diff>
--- a/Experiments_1B/03_RecombinationOperators/Levi/curves.xlsx
+++ b/Experiments_1B/03_RecombinationOperators/Levi/curves.xlsx
@@ -444,10 +444,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.425349760878878</v>
+        <v>0.4921137632341332</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4287885932748355</v>
+        <v>0.4169217266296197</v>
       </c>
     </row>
     <row r="3">
@@ -455,10 +455,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3086145413472978</v>
+        <v>0.3577899246459215</v>
       </c>
       <c r="C3" t="n">
-        <v>0.324186851759787</v>
+        <v>0.298156122963</v>
       </c>
     </row>
     <row r="4">
@@ -466,10 +466,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2579516118744265</v>
+        <v>0.2656824559673652</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2847374100086431</v>
+        <v>0.255375722610401</v>
       </c>
     </row>
     <row r="5">
@@ -477,10 +477,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2267178472946126</v>
+        <v>0.2385099774292138</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2410692330919888</v>
+        <v>0.2137501517028597</v>
       </c>
     </row>
     <row r="6">
@@ -488,10 +488,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1801263400852565</v>
+        <v>0.2112135552401316</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1912634598934405</v>
+        <v>0.1982156937108346</v>
       </c>
     </row>
     <row r="7">
@@ -499,10 +499,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1690410313255293</v>
+        <v>0.1815427643486399</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1620784843944073</v>
+        <v>0.1680443809776023</v>
       </c>
     </row>
     <row r="8">
@@ -510,10 +510,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1506899010905188</v>
+        <v>0.1689107045739007</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1476669555899166</v>
+        <v>0.1537537631784035</v>
       </c>
     </row>
     <row r="9">
@@ -521,10 +521,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1405492111552641</v>
+        <v>0.1529334187846399</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1402957689764788</v>
+        <v>0.1429751495565622</v>
       </c>
     </row>
     <row r="10">
@@ -532,10 +532,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1304086182470028</v>
+        <v>0.1443050583985663</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1289101012145684</v>
+        <v>0.1384205724160394</v>
       </c>
     </row>
     <row r="11">
@@ -543,10 +543,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.125629236701751</v>
+        <v>0.1371307548973885</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1244008008416825</v>
+        <v>0.1298507594632819</v>
       </c>
     </row>
     <row r="12">
@@ -554,10 +554,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1187662955429383</v>
+        <v>0.1292130536748318</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1193238525191493</v>
+        <v>0.1222515002737651</v>
       </c>
     </row>
     <row r="13">
@@ -565,10 +565,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.114574534789643</v>
+        <v>0.1186860701110718</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1177488004712042</v>
+        <v>0.1186686613971801</v>
       </c>
     </row>
     <row r="14">
@@ -576,10 +576,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1079176904466566</v>
+        <v>0.1132925159321142</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1157673534191278</v>
+        <v>0.1127758394132703</v>
       </c>
     </row>
     <row r="15">
@@ -587,10 +587,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1025153153159739</v>
+        <v>0.1090158994085069</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1092627678688812</v>
+        <v>0.1083160460957825</v>
       </c>
     </row>
     <row r="16">
@@ -598,10 +598,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.09676412667185032</v>
+        <v>0.1031317163807108</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1010896888188235</v>
+        <v>0.1054678561349634</v>
       </c>
     </row>
     <row r="17">
@@ -609,10 +609,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.09432910890599434</v>
+        <v>0.0967708005088917</v>
       </c>
       <c r="C17" t="n">
-        <v>0.09689976693509199</v>
+        <v>0.1017412894218696</v>
       </c>
     </row>
     <row r="18">
@@ -620,10 +620,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.09322480705033015</v>
+        <v>0.09558944583013872</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0935877580634446</v>
+        <v>0.0957630032429886</v>
       </c>
     </row>
     <row r="19">
@@ -631,10 +631,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.08368409409658552</v>
+        <v>0.08972353266357613</v>
       </c>
       <c r="C19" t="n">
-        <v>0.09124191239941803</v>
+        <v>0.09351025577644716</v>
       </c>
     </row>
     <row r="20">
@@ -642,10 +642,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0804519673456152</v>
+        <v>0.08763284846260272</v>
       </c>
       <c r="C20" t="n">
-        <v>0.08807715131177733</v>
+        <v>0.09206580421127608</v>
       </c>
     </row>
     <row r="21">
@@ -653,10 +653,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0782450055688839</v>
+        <v>0.08521247588946658</v>
       </c>
       <c r="C21" t="n">
-        <v>0.08571741385142348</v>
+        <v>0.09137771212763178</v>
       </c>
     </row>
     <row r="22">
@@ -664,10 +664,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0780173663003513</v>
+        <v>0.08146218193997859</v>
       </c>
       <c r="C22" t="n">
-        <v>0.08366714737334505</v>
+        <v>0.08987096412353507</v>
       </c>
     </row>
     <row r="23">
@@ -675,10 +675,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.0769596432578372</v>
+        <v>0.07915353347298926</v>
       </c>
       <c r="C23" t="n">
-        <v>0.08033059206805515</v>
+        <v>0.0864543172634996</v>
       </c>
     </row>
     <row r="24">
@@ -686,10 +686,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.07684036133309249</v>
+        <v>0.07509397477822893</v>
       </c>
       <c r="C24" t="n">
-        <v>0.07560372003540775</v>
+        <v>0.08183111747933333</v>
       </c>
     </row>
     <row r="25">
@@ -697,10 +697,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.07565110764615589</v>
+        <v>0.07085496947384164</v>
       </c>
       <c r="C25" t="n">
-        <v>0.07183854580743489</v>
+        <v>0.07381985018172213</v>
       </c>
     </row>
     <row r="26">
@@ -708,10 +708,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.07416116745291595</v>
+        <v>0.07085496947384164</v>
       </c>
       <c r="C26" t="n">
-        <v>0.06706491487870517</v>
+        <v>0.06986000963357868</v>
       </c>
     </row>
     <row r="27">
@@ -719,10 +719,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.07315218739345598</v>
+        <v>0.06809771667965428</v>
       </c>
       <c r="C27" t="n">
-        <v>0.06631896599558929</v>
+        <v>0.0694582205563456</v>
       </c>
     </row>
     <row r="28">
@@ -730,10 +730,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.06978558249721173</v>
+        <v>0.06655998685352991</v>
       </c>
       <c r="C28" t="n">
-        <v>0.06499310223860987</v>
+        <v>0.0638220904672631</v>
       </c>
     </row>
     <row r="29">
@@ -741,10 +741,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.06783081359283039</v>
+        <v>0.06381233515971264</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0630723081376932</v>
+        <v>0.05925940212865974</v>
       </c>
     </row>
     <row r="30">
@@ -752,10 +752,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.06617856292713319</v>
+        <v>0.06058627212454876</v>
       </c>
       <c r="C30" t="n">
-        <v>0.059353806501436</v>
+        <v>0.05925940212865974</v>
       </c>
     </row>
     <row r="31">
@@ -763,10 +763,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.06471547072411625</v>
+        <v>0.05825796053590906</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0584447028966024</v>
+        <v>0.05791309011602975</v>
       </c>
     </row>
     <row r="32">
@@ -774,10 +774,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.06063321574038063</v>
+        <v>0.05727388728547941</v>
       </c>
       <c r="C32" t="n">
-        <v>0.05585295155250578</v>
+        <v>0.05424219984535979</v>
       </c>
     </row>
     <row r="33">
@@ -785,10 +785,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.05920353723680675</v>
+        <v>0.05495858666691012</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0532149401245774</v>
+        <v>0.0525427657955628</v>
       </c>
     </row>
     <row r="34">
@@ -796,10 +796,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.05728767288273694</v>
+        <v>0.05256176313599795</v>
       </c>
       <c r="C34" t="n">
-        <v>0.05229413313204986</v>
+        <v>0.04967757523351792</v>
       </c>
     </row>
     <row r="35">
@@ -807,10 +807,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.05529266423456201</v>
+        <v>0.0514805590245028</v>
       </c>
       <c r="C35" t="n">
-        <v>0.04895929949470713</v>
+        <v>0.04892949502963228</v>
       </c>
     </row>
     <row r="36">
@@ -818,10 +818,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.05352775480048343</v>
+        <v>0.0502304870057523</v>
       </c>
       <c r="C36" t="n">
-        <v>0.04895929949470713</v>
+        <v>0.04760220410926243</v>
       </c>
     </row>
     <row r="37">
@@ -829,10 +829,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.04940300585326265</v>
+        <v>0.04872973502770343</v>
       </c>
       <c r="C37" t="n">
-        <v>0.04702054305625716</v>
+        <v>0.04732590703235756</v>
       </c>
     </row>
     <row r="38">
@@ -840,10 +840,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.04680352548756619</v>
+        <v>0.04798369865694212</v>
       </c>
       <c r="C38" t="n">
-        <v>0.04623029860841853</v>
+        <v>0.04558075006807642</v>
       </c>
     </row>
     <row r="39">
@@ -851,10 +851,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.04557306903496072</v>
+        <v>0.04662972785691528</v>
       </c>
       <c r="C39" t="n">
-        <v>0.04396332707869043</v>
+        <v>0.04455066105846337</v>
       </c>
     </row>
     <row r="40">
@@ -862,10 +862,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.04477598264090231</v>
+        <v>0.04630578967593778</v>
       </c>
       <c r="C40" t="n">
-        <v>0.04280354856857418</v>
+        <v>0.04389954535734883</v>
       </c>
     </row>
     <row r="41">
@@ -873,10 +873,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.04398788556632183</v>
+        <v>0.04203629737015371</v>
       </c>
       <c r="C41" t="n">
-        <v>0.04130201975446966</v>
+        <v>0.04303937913414572</v>
       </c>
     </row>
     <row r="42">
@@ -884,10 +884,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0431210755507979</v>
+        <v>0.04058293106044514</v>
       </c>
       <c r="C42" t="n">
-        <v>0.03962363631084932</v>
+        <v>0.0418284677713139</v>
       </c>
     </row>
     <row r="43">
@@ -895,10 +895,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.04166646624570765</v>
+        <v>0.03996537422650535</v>
       </c>
       <c r="C43" t="n">
-        <v>0.03875938023347761</v>
+        <v>0.04018826358890272</v>
       </c>
     </row>
     <row r="44">
@@ -906,10 +906,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.04071377265468408</v>
+        <v>0.03996537422650535</v>
       </c>
       <c r="C44" t="n">
-        <v>0.03823293580880448</v>
+        <v>0.03994482338295072</v>
       </c>
     </row>
     <row r="45">
@@ -917,10 +917,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.03949215190573079</v>
+        <v>0.03811822082374972</v>
       </c>
       <c r="C45" t="n">
-        <v>0.03823293580880448</v>
+        <v>0.03971277869605718</v>
       </c>
     </row>
     <row r="46">
@@ -928,10 +928,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.03939488888198336</v>
+        <v>0.03636438481181088</v>
       </c>
       <c r="C46" t="n">
-        <v>0.03648230027229914</v>
+        <v>0.03690913724918352</v>
       </c>
     </row>
     <row r="47">
@@ -939,10 +939,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.03932185422309174</v>
+        <v>0.0356594020389015</v>
       </c>
       <c r="C47" t="n">
-        <v>0.03538468532103555</v>
+        <v>0.03673049624419825</v>
       </c>
     </row>
     <row r="48">
@@ -950,10 +950,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.03814752045072598</v>
+        <v>0.0356594020389015</v>
       </c>
       <c r="C48" t="n">
-        <v>0.03455340772628556</v>
+        <v>0.03597313939345415</v>
       </c>
     </row>
     <row r="49">
@@ -961,10 +961,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.03721928685470519</v>
+        <v>0.0356594020389015</v>
       </c>
       <c r="C49" t="n">
-        <v>0.03390481889475596</v>
+        <v>0.03491588429121553</v>
       </c>
     </row>
     <row r="50">
@@ -972,10 +972,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.03619413131052906</v>
+        <v>0.03479910853269602</v>
       </c>
       <c r="C50" t="n">
-        <v>0.03372695649673714</v>
+        <v>0.03458766967838225</v>
       </c>
     </row>
     <row r="51">
@@ -983,10 +983,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.03591446692834559</v>
+        <v>0.03390444274861265</v>
       </c>
       <c r="C51" t="n">
-        <v>0.03188240221945571</v>
+        <v>0.03458766967838225</v>
       </c>
     </row>
     <row r="52">
@@ -994,10 +994,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.03522448932233128</v>
+        <v>0.03169587465594961</v>
       </c>
       <c r="C52" t="n">
-        <v>0.03160878997949618</v>
+        <v>0.03342439717364731</v>
       </c>
     </row>
     <row r="53">
@@ -1005,10 +1005,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.03486224615187014</v>
+        <v>0.03073941848397484</v>
       </c>
       <c r="C53" t="n">
-        <v>0.03128038042470283</v>
+        <v>0.03337489600206536</v>
       </c>
     </row>
     <row r="54">
@@ -1016,10 +1016,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.03481441702323654</v>
+        <v>0.02895003505702824</v>
       </c>
       <c r="C54" t="n">
-        <v>0.03128038042470283</v>
+        <v>0.03164652248489488</v>
       </c>
     </row>
     <row r="55">
@@ -1027,10 +1027,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.03446477595274789</v>
+        <v>0.02767096663749147</v>
       </c>
       <c r="C55" t="n">
-        <v>0.03122966269001591</v>
+        <v>0.02971006822102542</v>
       </c>
     </row>
     <row r="56">
@@ -1038,10 +1038,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.03332644676929308</v>
+        <v>0.02698217007308368</v>
       </c>
       <c r="C56" t="n">
-        <v>0.03030852572564135</v>
+        <v>0.02952245753757781</v>
       </c>
     </row>
     <row r="57">
@@ -1049,10 +1049,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.03269281545039335</v>
+        <v>0.02697885760097215</v>
       </c>
       <c r="C57" t="n">
-        <v>0.03020103178357823</v>
+        <v>0.02908598035304358</v>
       </c>
     </row>
     <row r="58">
@@ -1060,10 +1060,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.03237425862709915</v>
+        <v>0.02689269670489793</v>
       </c>
       <c r="C58" t="n">
-        <v>0.02919544264585557</v>
+        <v>0.02732380190648503</v>
       </c>
     </row>
     <row r="59">
@@ -1071,10 +1071,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.03206967554750417</v>
+        <v>0.02672296321903753</v>
       </c>
       <c r="C59" t="n">
-        <v>0.02847537127167453</v>
+        <v>0.02701227760734876</v>
       </c>
     </row>
     <row r="60">
@@ -1082,10 +1082,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0313527282017655</v>
+        <v>0.02649722694453633</v>
       </c>
       <c r="C60" t="n">
-        <v>0.02847537127167453</v>
+        <v>0.02585863187639698</v>
       </c>
     </row>
     <row r="61">
@@ -1093,10 +1093,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0306545570798267</v>
+        <v>0.02567916495106673</v>
       </c>
       <c r="C61" t="n">
-        <v>0.02811095299392043</v>
+        <v>0.02505639635372614</v>
       </c>
     </row>
     <row r="62">
@@ -1104,10 +1104,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.02959852633708611</v>
+        <v>0.02548674285071286</v>
       </c>
       <c r="C62" t="n">
-        <v>0.02694575884250817</v>
+        <v>0.02503761305188836</v>
       </c>
     </row>
     <row r="63">
@@ -1115,10 +1115,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.02896143077788739</v>
+        <v>0.02535472974727012</v>
       </c>
       <c r="C63" t="n">
-        <v>0.02620222202155591</v>
+        <v>0.02485221541582991</v>
       </c>
     </row>
     <row r="64">
@@ -1126,10 +1126,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.02702136840497154</v>
+        <v>0.02491026188747057</v>
       </c>
       <c r="C64" t="n">
-        <v>0.026099233455011</v>
+        <v>0.02454045985334723</v>
       </c>
     </row>
     <row r="65">
@@ -1137,10 +1137,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.02647870065013861</v>
+        <v>0.02451668836223663</v>
       </c>
       <c r="C65" t="n">
-        <v>0.02520648961028955</v>
+        <v>0.02454045985334723</v>
       </c>
     </row>
     <row r="66">
@@ -1148,10 +1148,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.0251797351747748</v>
+        <v>0.02420792609073473</v>
       </c>
       <c r="C66" t="n">
-        <v>0.02484355997680153</v>
+        <v>0.02452554849848186</v>
       </c>
     </row>
     <row r="67">
@@ -1159,10 +1159,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.02505734542625927</v>
+        <v>0.02385533901305421</v>
       </c>
       <c r="C67" t="n">
-        <v>0.02447570789553048</v>
+        <v>0.02234530551582203</v>
       </c>
     </row>
     <row r="68">
@@ -1170,10 +1170,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.0248917616813506</v>
+        <v>0.02355193200415924</v>
       </c>
       <c r="C68" t="n">
-        <v>0.02374190770684135</v>
+        <v>0.02217713872980349</v>
       </c>
     </row>
     <row r="69">
@@ -1181,10 +1181,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.02401329292550914</v>
+        <v>0.02320922755719274</v>
       </c>
       <c r="C69" t="n">
-        <v>0.0234609518307144</v>
+        <v>0.02132532539957563</v>
       </c>
     </row>
     <row r="70">
@@ -1192,10 +1192,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.02352886268059494</v>
+        <v>0.02320922755719274</v>
       </c>
       <c r="C70" t="n">
-        <v>0.0234609518307144</v>
+        <v>0.020929248284103</v>
       </c>
     </row>
     <row r="71">
@@ -1203,10 +1203,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.02283634813883315</v>
+        <v>0.02286439606567239</v>
       </c>
       <c r="C71" t="n">
-        <v>0.02226012728335603</v>
+        <v>0.02081664271684451</v>
       </c>
     </row>
     <row r="72">
@@ -1214,10 +1214,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.02237413092796449</v>
+        <v>0.02260936515314114</v>
       </c>
       <c r="C72" t="n">
-        <v>0.02136116180195497</v>
+        <v>0.02034847877994338</v>
       </c>
     </row>
     <row r="73">
@@ -1225,10 +1225,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.02135983070945062</v>
+        <v>0.02216751177631602</v>
       </c>
       <c r="C73" t="n">
-        <v>0.02056086736884525</v>
+        <v>0.01994851326975382</v>
       </c>
     </row>
     <row r="74">
@@ -1236,10 +1236,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.02124666199632341</v>
+        <v>0.02128447706651507</v>
       </c>
       <c r="C74" t="n">
-        <v>0.02056086736884525</v>
+        <v>0.01983124417144487</v>
       </c>
     </row>
     <row r="75">
@@ -1247,10 +1247,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.02098321952660996</v>
+        <v>0.02082862046204376</v>
       </c>
       <c r="C75" t="n">
-        <v>0.01985308384068276</v>
+        <v>0.01981874442312572</v>
       </c>
     </row>
     <row r="76">
@@ -1258,10 +1258,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.02041636330787882</v>
+        <v>0.01974584598273181</v>
       </c>
       <c r="C76" t="n">
-        <v>0.0197667067029524</v>
+        <v>0.01947501913552337</v>
       </c>
     </row>
     <row r="77">
@@ -1269,10 +1269,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.01995151177792211</v>
+        <v>0.01956920673330419</v>
       </c>
       <c r="C77" t="n">
-        <v>0.01886460362050942</v>
+        <v>0.01891344624138968</v>
       </c>
     </row>
     <row r="78">
@@ -1280,10 +1280,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.01982551045582878</v>
+        <v>0.01926353389375936</v>
       </c>
       <c r="C78" t="n">
-        <v>0.0185851121333764</v>
+        <v>0.0188717583883589</v>
       </c>
     </row>
     <row r="79">
@@ -1291,10 +1291,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.01904856704942238</v>
+        <v>0.01898545588108762</v>
       </c>
       <c r="C79" t="n">
-        <v>0.01827373533972007</v>
+        <v>0.01865689006277217</v>
       </c>
     </row>
     <row r="80">
@@ -1302,10 +1302,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.01846979564604085</v>
+        <v>0.01896553385178651</v>
       </c>
       <c r="C80" t="n">
-        <v>0.01752103895836717</v>
+        <v>0.01806184913357425</v>
       </c>
     </row>
     <row r="81">
@@ -1313,10 +1313,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.01838304773223407</v>
+        <v>0.01873175680614025</v>
       </c>
       <c r="C81" t="n">
-        <v>0.01728630890257617</v>
+        <v>0.01806184913357425</v>
       </c>
     </row>
     <row r="82">
@@ -1324,10 +1324,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.0182404129305073</v>
+        <v>0.01766993073390073</v>
       </c>
       <c r="C82" t="n">
-        <v>0.01725245187121712</v>
+        <v>0.0177952198494039</v>
       </c>
     </row>
     <row r="83">
@@ -1335,10 +1335,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.01799912400365629</v>
+        <v>0.01702881577989464</v>
       </c>
       <c r="C83" t="n">
-        <v>0.01601724211015921</v>
+        <v>0.01703673571601444</v>
       </c>
     </row>
     <row r="84">
@@ -1346,10 +1346,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.01759690831264692</v>
+        <v>0.01590911282509776</v>
       </c>
       <c r="C84" t="n">
-        <v>0.01536533394789359</v>
+        <v>0.01646906780697488</v>
       </c>
     </row>
     <row r="85">
@@ -1357,10 +1357,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.01676494734618149</v>
+        <v>0.01360279409158881</v>
       </c>
       <c r="C85" t="n">
-        <v>0.01489541316726797</v>
+        <v>0.01638810509400009</v>
       </c>
     </row>
     <row r="86">
@@ -1368,10 +1368,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.01659558916358688</v>
+        <v>0.01360279409158881</v>
       </c>
       <c r="C86" t="n">
-        <v>0.01436484362958649</v>
+        <v>0.01599548393136765</v>
       </c>
     </row>
     <row r="87">
@@ -1379,10 +1379,10 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.01653864155197853</v>
+        <v>0.01356471385622591</v>
       </c>
       <c r="C87" t="n">
-        <v>0.01436003313855989</v>
+        <v>0.0158428594965193</v>
       </c>
     </row>
     <row r="88">
@@ -1390,10 +1390,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.01653864155197853</v>
+        <v>0.01356471385622591</v>
       </c>
       <c r="C88" t="n">
-        <v>0.01367414818653847</v>
+        <v>0.01558071257031202</v>
       </c>
     </row>
     <row r="89">
@@ -1401,10 +1401,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.01614708120957771</v>
+        <v>0.01356471385622591</v>
       </c>
       <c r="C89" t="n">
-        <v>0.01351016903998647</v>
+        <v>0.01521935002393227</v>
       </c>
     </row>
     <row r="90">
@@ -1412,10 +1412,10 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.01602157485678973</v>
+        <v>0.01349603707731911</v>
       </c>
       <c r="C90" t="n">
-        <v>0.01317547489245732</v>
+        <v>0.01521935002393227</v>
       </c>
     </row>
     <row r="91">
@@ -1423,10 +1423,10 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.01585631107739848</v>
+        <v>0.01326546468420888</v>
       </c>
       <c r="C91" t="n">
-        <v>0.0121859666404535</v>
+        <v>0.01521935002393227</v>
       </c>
     </row>
     <row r="92">
@@ -1434,10 +1434,10 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.01518959642473993</v>
+        <v>0.0130606504853824</v>
       </c>
       <c r="C92" t="n">
-        <v>0.01155100004227987</v>
+        <v>0.01512226036527487</v>
       </c>
     </row>
     <row r="93">
@@ -1445,10 +1445,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.01498852328709616</v>
+        <v>0.01296160635096371</v>
       </c>
       <c r="C93" t="n">
-        <v>0.01139416259943731</v>
+        <v>0.01512226036527487</v>
       </c>
     </row>
     <row r="94">
@@ -1456,10 +1456,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.0143376236227183</v>
+        <v>0.01207487447882333</v>
       </c>
       <c r="C94" t="n">
-        <v>0.01123495704520763</v>
+        <v>0.01484032387108157</v>
       </c>
     </row>
     <row r="95">
@@ -1467,10 +1467,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.01428274459222899</v>
+        <v>0.01188040963067557</v>
       </c>
       <c r="C95" t="n">
-        <v>0.01120252973314415</v>
+        <v>0.01467406244535064</v>
       </c>
     </row>
     <row r="96">
@@ -1478,10 +1478,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.01367412516273939</v>
+        <v>0.01188040963067557</v>
       </c>
       <c r="C96" t="n">
-        <v>0.01116921995153361</v>
+        <v>0.01464585347234515</v>
       </c>
     </row>
     <row r="97">
@@ -1489,10 +1489,10 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.01347526612020409</v>
+        <v>0.01178830361240183</v>
       </c>
       <c r="C97" t="n">
-        <v>0.01110222080517428</v>
+        <v>0.01461306785800283</v>
       </c>
     </row>
     <row r="98">
@@ -1500,10 +1500,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.01310855960614738</v>
+        <v>0.01153775688829073</v>
       </c>
       <c r="C98" t="n">
-        <v>0.01061769841917268</v>
+        <v>0.01419431523053593</v>
       </c>
     </row>
     <row r="99">
@@ -1511,10 +1511,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.01283956219012114</v>
+        <v>0.01149306067961372</v>
       </c>
       <c r="C99" t="n">
-        <v>0.01035962211670875</v>
+        <v>0.01404582296539805</v>
       </c>
     </row>
     <row r="100">
@@ -1522,10 +1522,10 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.0127022861579466</v>
+        <v>0.01092057073354118</v>
       </c>
       <c r="C100" t="n">
-        <v>0.01005633012305492</v>
+        <v>0.01404582296539805</v>
       </c>
     </row>
     <row r="101">
@@ -1533,10 +1533,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.01265709018713026</v>
+        <v>0.01085118172299611</v>
       </c>
       <c r="C101" t="n">
-        <v>0.0100209078241799</v>
+        <v>0.01359242044170766</v>
       </c>
     </row>
     <row r="102">
@@ -1544,10 +1544,10 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0.01265038379745767</v>
+        <v>0.01014973276848298</v>
       </c>
       <c r="C102" t="n">
-        <v>0.009908477698099662</v>
+        <v>0.01357289566102517</v>
       </c>
     </row>
     <row r="103">
@@ -1555,10 +1555,10 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.01256948760251067</v>
+        <v>0.009760661661502733</v>
       </c>
       <c r="C103" t="n">
-        <v>0.009827398686260896</v>
+        <v>0.01340391928627417</v>
       </c>
     </row>
     <row r="104">
@@ -1566,10 +1566,10 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.01253036590978897</v>
+        <v>0.009650997264362702</v>
       </c>
       <c r="C104" t="n">
-        <v>0.009682162105219693</v>
+        <v>0.01340391928627417</v>
       </c>
     </row>
     <row r="105">
@@ -1577,10 +1577,10 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.01227540244775178</v>
+        <v>0.009624809887914025</v>
       </c>
       <c r="C105" t="n">
-        <v>0.009664157511994001</v>
+        <v>0.01306717565941909</v>
       </c>
     </row>
     <row r="106">
@@ -1588,10 +1588,10 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.01185946372286092</v>
+        <v>0.009439294940926785</v>
       </c>
       <c r="C106" t="n">
-        <v>0.009197247294028866</v>
+        <v>0.01285661075161139</v>
       </c>
     </row>
     <row r="107">
@@ -1599,10 +1599,10 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.0118361413081938</v>
+        <v>0.00927133760477054</v>
       </c>
       <c r="C107" t="n">
-        <v>0.009197247294028866</v>
+        <v>0.01279454629419289</v>
       </c>
     </row>
     <row r="108">
@@ -1610,10 +1610,10 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.01137579187437303</v>
+        <v>0.009098173083351202</v>
       </c>
       <c r="C108" t="n">
-        <v>0.009150713077470084</v>
+        <v>0.01210500444074052</v>
       </c>
     </row>
     <row r="109">
@@ -1621,10 +1621,10 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.0112341335353582</v>
+        <v>0.008990075086068439</v>
       </c>
       <c r="C109" t="n">
-        <v>0.008802733525666748</v>
+        <v>0.01151374083078534</v>
       </c>
     </row>
     <row r="110">
@@ -1632,10 +1632,10 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0.01111847027524418</v>
+        <v>0.008572984619451081</v>
       </c>
       <c r="C110" t="n">
-        <v>0.008675390320292173</v>
+        <v>0.0110603981557037</v>
       </c>
     </row>
     <row r="111">
@@ -1643,10 +1643,10 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0.0108013395877998</v>
+        <v>0.00853253009634038</v>
       </c>
       <c r="C111" t="n">
-        <v>0.008633698045202802</v>
+        <v>0.01075871431161922</v>
       </c>
     </row>
     <row r="112">
@@ -1654,10 +1654,10 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.01069492615021603</v>
+        <v>0.00853253009634038</v>
       </c>
       <c r="C112" t="n">
-        <v>0.008633698045202802</v>
+        <v>0.01018675622990938</v>
       </c>
     </row>
     <row r="113">
@@ -1665,10 +1665,10 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.01022833527488435</v>
+        <v>0.008291481580255866</v>
       </c>
       <c r="C113" t="n">
-        <v>0.00850142126949947</v>
+        <v>0.01016575818309094</v>
       </c>
     </row>
     <row r="114">
@@ -1676,10 +1676,10 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.009837723282619034</v>
+        <v>0.007919217680734192</v>
       </c>
       <c r="C114" t="n">
-        <v>0.00850142126949947</v>
+        <v>0.00990960735883329</v>
       </c>
     </row>
     <row r="115">
@@ -1687,10 +1687,10 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.009760850927952477</v>
+        <v>0.007919217680734192</v>
       </c>
       <c r="C115" t="n">
-        <v>0.007723710532010933</v>
+        <v>0.009708060119638717</v>
       </c>
     </row>
     <row r="116">
@@ -1698,10 +1698,10 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0.009162026085937044</v>
+        <v>0.0076312564945713</v>
       </c>
       <c r="C116" t="n">
-        <v>0.007723710532010933</v>
+        <v>0.009466471272319942</v>
       </c>
     </row>
     <row r="117">
@@ -1709,10 +1709,10 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0.008744895986896756</v>
+        <v>0.007574394524029877</v>
       </c>
       <c r="C117" t="n">
-        <v>0.007716268086701776</v>
+        <v>0.008991763990255896</v>
       </c>
     </row>
     <row r="118">
@@ -1720,10 +1720,10 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0.008572880111815343</v>
+        <v>0.007429181240790657</v>
       </c>
       <c r="C118" t="n">
-        <v>0.00745421735570992</v>
+        <v>0.00890172701283885</v>
       </c>
     </row>
     <row r="119">
@@ -1731,10 +1731,10 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>0.008404105505936831</v>
+        <v>0.007427182696204647</v>
       </c>
       <c r="C119" t="n">
-        <v>0.007431086099806302</v>
+        <v>0.008827618287635879</v>
       </c>
     </row>
     <row r="120">
@@ -1742,10 +1742,10 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0.008404105505936831</v>
+        <v>0.007321888839849132</v>
       </c>
       <c r="C120" t="n">
-        <v>0.007390762223401418</v>
+        <v>0.008764566653585175</v>
       </c>
     </row>
     <row r="121">
@@ -1753,10 +1753,10 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>0.008213287527975064</v>
+        <v>0.007096489386389103</v>
       </c>
       <c r="C121" t="n">
-        <v>0.007362363637629096</v>
+        <v>0.008745747582480203</v>
       </c>
     </row>
     <row r="122">
@@ -1764,10 +1764,10 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>0.00817999656924503</v>
+        <v>0.007045147091212215</v>
       </c>
       <c r="C122" t="n">
-        <v>0.007187319811903407</v>
+        <v>0.008510203162420722</v>
       </c>
     </row>
     <row r="123">
@@ -1775,10 +1775,10 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>0.00817999656924503</v>
+        <v>0.006711767283242188</v>
       </c>
       <c r="C123" t="n">
-        <v>0.007187319811903407</v>
+        <v>0.008376361029352535</v>
       </c>
     </row>
     <row r="124">
@@ -1786,10 +1786,10 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>0.008018139337558598</v>
+        <v>0.006476978298331385</v>
       </c>
       <c r="C124" t="n">
-        <v>0.007156804703028573</v>
+        <v>0.008104481402096126</v>
       </c>
     </row>
     <row r="125">
@@ -1797,10 +1797,10 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.008018139337558598</v>
+        <v>0.006476978298331385</v>
       </c>
       <c r="C125" t="n">
-        <v>0.007038505880135083</v>
+        <v>0.008015112665342211</v>
       </c>
     </row>
     <row r="126">
@@ -1808,10 +1808,10 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.007668215781131651</v>
+        <v>0.006365784721857364</v>
       </c>
       <c r="C126" t="n">
-        <v>0.006907287029545911</v>
+        <v>0.008015112665342211</v>
       </c>
     </row>
     <row r="127">
@@ -1819,10 +1819,10 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.007437148188220256</v>
+        <v>0.005973495005963244</v>
       </c>
       <c r="C127" t="n">
-        <v>0.006800979110563251</v>
+        <v>0.007924487631682933</v>
       </c>
     </row>
     <row r="128">
@@ -1830,10 +1830,10 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.007366041983723461</v>
+        <v>0.005821475467351006</v>
       </c>
       <c r="C128" t="n">
-        <v>0.006784852876664416</v>
+        <v>0.007840415341385016</v>
       </c>
     </row>
     <row r="129">
@@ -1841,10 +1841,10 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.007292504827048969</v>
+        <v>0.005821475467351006</v>
       </c>
       <c r="C129" t="n">
-        <v>0.006732946052369023</v>
+        <v>0.007735987348881495</v>
       </c>
     </row>
     <row r="130">
@@ -1852,10 +1852,10 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.007274881957723975</v>
+        <v>0.005755609879960464</v>
       </c>
       <c r="C130" t="n">
-        <v>0.006613999584286268</v>
+        <v>0.007735987348881495</v>
       </c>
     </row>
     <row r="131">
@@ -1863,10 +1863,10 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0.006842099919254403</v>
+        <v>0.005755609879960464</v>
       </c>
       <c r="C131" t="n">
-        <v>0.006595394591497996</v>
+        <v>0.007735987348881495</v>
       </c>
     </row>
     <row r="132">
@@ -1874,10 +1874,10 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0.006797279451360157</v>
+        <v>0.005560990707733761</v>
       </c>
       <c r="C132" t="n">
-        <v>0.006385861002891073</v>
+        <v>0.007735987348881495</v>
       </c>
     </row>
     <row r="133">
@@ -1885,10 +1885,10 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>0.006584782056293034</v>
+        <v>0.005365760438316314</v>
       </c>
       <c r="C133" t="n">
-        <v>0.005923336010465883</v>
+        <v>0.00737438673177743</v>
       </c>
     </row>
     <row r="134">
@@ -1896,10 +1896,10 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>0.006584782056293034</v>
+        <v>0.005343145986415383</v>
       </c>
       <c r="C134" t="n">
-        <v>0.005923336010465883</v>
+        <v>0.00737438673177743</v>
       </c>
     </row>
     <row r="135">
@@ -1907,10 +1907,10 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>0.006546753731531915</v>
+        <v>0.005249506694395912</v>
       </c>
       <c r="C135" t="n">
-        <v>0.00585693251493596</v>
+        <v>0.007358841267231715</v>
       </c>
     </row>
     <row r="136">
@@ -1918,10 +1918,10 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>0.006492171399352146</v>
+        <v>0.005080114069807759</v>
       </c>
       <c r="C136" t="n">
-        <v>0.005690528961449587</v>
+        <v>0.007292635572795584</v>
       </c>
     </row>
     <row r="137">
@@ -1929,10 +1929,10 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0.006374724591581703</v>
+        <v>0.005020681437662325</v>
       </c>
       <c r="C137" t="n">
-        <v>0.005690528961449587</v>
+        <v>0.007159215479739071</v>
       </c>
     </row>
     <row r="138">
@@ -1940,10 +1940,10 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0.005917567723048845</v>
+        <v>0.005002726842206989</v>
       </c>
       <c r="C138" t="n">
-        <v>0.005549489511340417</v>
+        <v>0.00704516343431219</v>
       </c>
     </row>
     <row r="139">
@@ -1951,10 +1951,10 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.005532307653002923</v>
+        <v>0.004867992494538459</v>
       </c>
       <c r="C139" t="n">
-        <v>0.005549489511340417</v>
+        <v>0.007042694454027814</v>
       </c>
     </row>
     <row r="140">
@@ -1962,10 +1962,10 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.005252482099110179</v>
+        <v>0.004677310397215975</v>
       </c>
       <c r="C140" t="n">
-        <v>0.005430795923027907</v>
+        <v>0.006979911181032023</v>
       </c>
     </row>
     <row r="141">
@@ -1973,10 +1973,10 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.005186966852122117</v>
+        <v>0.004677310397215975</v>
       </c>
       <c r="C141" t="n">
-        <v>0.005430795923027907</v>
+        <v>0.006968763915531329</v>
       </c>
     </row>
     <row r="142">
@@ -1984,10 +1984,10 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.005122897970722204</v>
+        <v>0.004622471926653226</v>
       </c>
       <c r="C142" t="n">
-        <v>0.005243981034107058</v>
+        <v>0.006781751204624122</v>
       </c>
     </row>
     <row r="143">
@@ -1995,10 +1995,10 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0.004662248656024486</v>
+        <v>0.004485261524085789</v>
       </c>
       <c r="C143" t="n">
-        <v>0.005231998700639109</v>
+        <v>0.006781751204624122</v>
       </c>
     </row>
     <row r="144">
@@ -2006,10 +2006,10 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>0.00460198170357708</v>
+        <v>0.00429257853720846</v>
       </c>
       <c r="C144" t="n">
-        <v>0.005031500410221329</v>
+        <v>0.006731639654939062</v>
       </c>
     </row>
     <row r="145">
@@ -2017,10 +2017,10 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>0.004524990343502819</v>
+        <v>0.004136383879505189</v>
       </c>
       <c r="C145" t="n">
-        <v>0.004877452266944967</v>
+        <v>0.006464419832906461</v>
       </c>
     </row>
     <row r="146">
@@ -2028,10 +2028,10 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0.004368439624802731</v>
+        <v>0.004110548740549548</v>
       </c>
       <c r="C146" t="n">
-        <v>0.004871841168182366</v>
+        <v>0.006412990052159045</v>
       </c>
     </row>
     <row r="147">
@@ -2039,10 +2039,10 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0.004368439624802731</v>
+        <v>0.004010611427597405</v>
       </c>
       <c r="C147" t="n">
-        <v>0.00470940879527291</v>
+        <v>0.006116123665321528</v>
       </c>
     </row>
     <row r="148">
@@ -2050,10 +2050,10 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.004368439624802731</v>
+        <v>0.003958130546751618</v>
       </c>
       <c r="C148" t="n">
-        <v>0.004531520399681746</v>
+        <v>0.006032782522988914</v>
       </c>
     </row>
     <row r="149">
@@ -2061,10 +2061,10 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0.004250871033662706</v>
+        <v>0.003951668314925451</v>
       </c>
       <c r="C149" t="n">
-        <v>0.004503069829476455</v>
+        <v>0.006032782522988914</v>
       </c>
     </row>
     <row r="150">
@@ -2072,10 +2072,10 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0.004094569423825672</v>
+        <v>0.003869410837455503</v>
       </c>
       <c r="C150" t="n">
-        <v>0.004490834371657386</v>
+        <v>0.006032782522988914</v>
       </c>
     </row>
     <row r="151">
@@ -2083,10 +2083,10 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.004094569423825672</v>
+        <v>0.003869410837455503</v>
       </c>
       <c r="C151" t="n">
-        <v>0.004260992205110401</v>
+        <v>0.005928650848152692</v>
       </c>
     </row>
     <row r="152">
@@ -2094,10 +2094,10 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.004064113071702909</v>
+        <v>0.00380643878311715</v>
       </c>
       <c r="C152" t="n">
-        <v>0.004260992205110401</v>
+        <v>0.005747044138199173</v>
       </c>
     </row>
     <row r="153">
@@ -2105,10 +2105,10 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0.004064113071702909</v>
+        <v>0.003627174613363695</v>
       </c>
       <c r="C153" t="n">
-        <v>0.004176777775144607</v>
+        <v>0.005734002669112774</v>
       </c>
     </row>
     <row r="154">
@@ -2116,10 +2116,10 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>0.004064113071702909</v>
+        <v>0.003627174613363695</v>
       </c>
       <c r="C154" t="n">
-        <v>0.004128099562284617</v>
+        <v>0.005568690275875123</v>
       </c>
     </row>
     <row r="155">
@@ -2127,10 +2127,10 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>0.003988277950031789</v>
+        <v>0.003551007120633857</v>
       </c>
       <c r="C155" t="n">
-        <v>0.004092062721976522</v>
+        <v>0.005552922229264782</v>
       </c>
     </row>
     <row r="156">
@@ -2138,10 +2138,10 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>0.003845218805936055</v>
+        <v>0.003538688410378477</v>
       </c>
       <c r="C156" t="n">
-        <v>0.003909216802936221</v>
+        <v>0.005552922229264782</v>
       </c>
     </row>
     <row r="157">
@@ -2149,10 +2149,10 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>0.003845218805936055</v>
+        <v>0.003538688410378477</v>
       </c>
       <c r="C157" t="n">
-        <v>0.003844097904032239</v>
+        <v>0.005482859474214849</v>
       </c>
     </row>
     <row r="158">
@@ -2160,10 +2160,10 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>0.003828985144817276</v>
+        <v>0.003538688410378477</v>
       </c>
       <c r="C158" t="n">
-        <v>0.003822987635066858</v>
+        <v>0.00519653435509649</v>
       </c>
     </row>
     <row r="159">
@@ -2171,10 +2171,10 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>0.003828985144817276</v>
+        <v>0.003477563451921713</v>
       </c>
       <c r="C159" t="n">
-        <v>0.003806628184454402</v>
+        <v>0.005090422430164451</v>
       </c>
     </row>
     <row r="160">
@@ -2182,10 +2182,10 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>0.003727946155592174</v>
+        <v>0.003477563451921713</v>
       </c>
       <c r="C160" t="n">
-        <v>0.003780544183351771</v>
+        <v>0.005010378286087818</v>
       </c>
     </row>
     <row r="161">
@@ -2193,10 +2193,10 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>0.003727946155592174</v>
+        <v>0.003385891821934865</v>
       </c>
       <c r="C161" t="n">
-        <v>0.003747018690841016</v>
+        <v>0.004726152717138457</v>
       </c>
     </row>
     <row r="162">
@@ -2204,10 +2204,10 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>0.003528671807273957</v>
+        <v>0.003365184295232229</v>
       </c>
       <c r="C162" t="n">
-        <v>0.003747018690841016</v>
+        <v>0.004598243366476711</v>
       </c>
     </row>
     <row r="163">
@@ -2215,10 +2215,10 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>0.003527309364631205</v>
+        <v>0.003331660359607092</v>
       </c>
       <c r="C163" t="n">
-        <v>0.003716303311384882</v>
+        <v>0.004546377675777402</v>
       </c>
     </row>
     <row r="164">
@@ -2226,10 +2226,10 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>0.003497546985844456</v>
+        <v>0.00326686782034427</v>
       </c>
       <c r="C164" t="n">
-        <v>0.003660041000602623</v>
+        <v>0.004521063109891296</v>
       </c>
     </row>
     <row r="165">
@@ -2237,10 +2237,10 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>0.003497546985844456</v>
+        <v>0.003128514091030954</v>
       </c>
       <c r="C165" t="n">
-        <v>0.003542111785363883</v>
+        <v>0.004387300682338047</v>
       </c>
     </row>
     <row r="166">
@@ -2248,10 +2248,10 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>0.003434606872454632</v>
+        <v>0.003031855225522197</v>
       </c>
       <c r="C166" t="n">
-        <v>0.003539560898058796</v>
+        <v>0.004372170236114508</v>
       </c>
     </row>
     <row r="167">
@@ -2259,10 +2259,10 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>0.003405225377962433</v>
+        <v>0.003014836907098348</v>
       </c>
       <c r="C167" t="n">
-        <v>0.003497160966891806</v>
+        <v>0.004323947505724745</v>
       </c>
     </row>
     <row r="168">
@@ -2270,10 +2270,10 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>0.003209302340257006</v>
+        <v>0.003014836907098348</v>
       </c>
       <c r="C168" t="n">
-        <v>0.003494743061904452</v>
+        <v>0.004264786853407211</v>
       </c>
     </row>
     <row r="169">
@@ -2281,10 +2281,10 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>0.003136976302161421</v>
+        <v>0.00296120230231881</v>
       </c>
       <c r="C169" t="n">
-        <v>0.003492302427053225</v>
+        <v>0.004132222639441531</v>
       </c>
     </row>
     <row r="170">
@@ -2292,10 +2292,10 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>0.0029635397676109</v>
+        <v>0.002956980951505131</v>
       </c>
       <c r="C170" t="n">
-        <v>0.003479816666840016</v>
+        <v>0.003939251082075426</v>
       </c>
     </row>
     <row r="171">
@@ -2303,10 +2303,10 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>0.002961111706341957</v>
+        <v>0.002930983019840446</v>
       </c>
       <c r="C171" t="n">
-        <v>0.003346229845806302</v>
+        <v>0.003774475041132704</v>
       </c>
     </row>
     <row r="172">
@@ -2314,10 +2314,10 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>0.00295178805521726</v>
+        <v>0.002930983019840446</v>
       </c>
       <c r="C172" t="n">
-        <v>0.003346229845806302</v>
+        <v>0.003622231746100552</v>
       </c>
     </row>
     <row r="173">
@@ -2325,10 +2325,10 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>0.002889287360707227</v>
+        <v>0.00290149814500861</v>
       </c>
       <c r="C173" t="n">
-        <v>0.003219386297977989</v>
+        <v>0.003509352132744907</v>
       </c>
     </row>
     <row r="174">
@@ -2336,10 +2336,10 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>0.002731424314190817</v>
+        <v>0.002894029772295629</v>
       </c>
       <c r="C174" t="n">
-        <v>0.003139582269564523</v>
+        <v>0.00342600429889407</v>
       </c>
     </row>
     <row r="175">
@@ -2347,10 +2347,10 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>0.002731424314190817</v>
+        <v>0.002646972994523635</v>
       </c>
       <c r="C175" t="n">
-        <v>0.003075303236584378</v>
+        <v>0.00342600429889407</v>
       </c>
     </row>
     <row r="176">
@@ -2358,10 +2358,10 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>0.002685788176563687</v>
+        <v>0.002505214752427824</v>
       </c>
       <c r="C176" t="n">
-        <v>0.002924957335919159</v>
+        <v>0.003314592572517549</v>
       </c>
     </row>
     <row r="177">
@@ -2369,10 +2369,10 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>0.002654378964977389</v>
+        <v>0.002505214752427824</v>
       </c>
       <c r="C177" t="n">
-        <v>0.002903352593080444</v>
+        <v>0.003297709807953874</v>
       </c>
     </row>
     <row r="178">
@@ -2380,10 +2380,10 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>0.002603816538406098</v>
+        <v>0.002505214752427824</v>
       </c>
       <c r="C178" t="n">
-        <v>0.002880254099210418</v>
+        <v>0.003271468684099417</v>
       </c>
     </row>
     <row r="179">
@@ -2391,10 +2391,10 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>0.002603816538406098</v>
+        <v>0.002505214752427824</v>
       </c>
       <c r="C179" t="n">
-        <v>0.00284878523764594</v>
+        <v>0.003187271588051976</v>
       </c>
     </row>
     <row r="180">
@@ -2402,10 +2402,10 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>0.002568626418172914</v>
+        <v>0.002499724317104198</v>
       </c>
       <c r="C180" t="n">
-        <v>0.002829128866062871</v>
+        <v>0.003187271588051976</v>
       </c>
     </row>
     <row r="181">
@@ -2413,10 +2413,10 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>0.002561573650346892</v>
+        <v>0.002499724317104198</v>
       </c>
       <c r="C181" t="n">
-        <v>0.002728095178505362</v>
+        <v>0.003140424391405641</v>
       </c>
     </row>
     <row r="182">
@@ -2424,10 +2424,10 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>0.002541161378461814</v>
+        <v>0.002437457018451287</v>
       </c>
       <c r="C182" t="n">
-        <v>0.002624834231391664</v>
+        <v>0.002995142619738251</v>
       </c>
     </row>
     <row r="183">
@@ -2435,10 +2435,10 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>0.00250099224962122</v>
+        <v>0.002437457018451287</v>
       </c>
       <c r="C183" t="n">
-        <v>0.002609214826548807</v>
+        <v>0.002915878660238435</v>
       </c>
     </row>
     <row r="184">
@@ -2446,10 +2446,10 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>0.00247259399859273</v>
+        <v>0.002400082208134183</v>
       </c>
       <c r="C184" t="n">
-        <v>0.002588903796904762</v>
+        <v>0.002906090704865563</v>
       </c>
     </row>
     <row r="185">
@@ -2457,10 +2457,10 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>0.002442859499557558</v>
+        <v>0.002398850027296707</v>
       </c>
       <c r="C185" t="n">
-        <v>0.002525783200716959</v>
+        <v>0.002782785948488516</v>
       </c>
     </row>
     <row r="186">
@@ -2468,10 +2468,10 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>0.002442859499557558</v>
+        <v>0.002357116915532946</v>
       </c>
       <c r="C186" t="n">
-        <v>0.002434090227388724</v>
+        <v>0.002778425146132879</v>
       </c>
     </row>
     <row r="187">
@@ -2479,10 +2479,10 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>0.002418355334496439</v>
+        <v>0.002320551093514516</v>
       </c>
       <c r="C187" t="n">
-        <v>0.002408776987128321</v>
+        <v>0.002736004409166479</v>
       </c>
     </row>
     <row r="188">
@@ -2490,10 +2490,10 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>0.002385871363498172</v>
+        <v>0.002241644820735717</v>
       </c>
       <c r="C188" t="n">
-        <v>0.002391708920886804</v>
+        <v>0.002654360125045338</v>
       </c>
     </row>
     <row r="189">
@@ -2501,10 +2501,10 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>0.002385871363498172</v>
+        <v>0.002240710461110857</v>
       </c>
       <c r="C189" t="n">
-        <v>0.002314356525099068</v>
+        <v>0.002488424939884523</v>
       </c>
     </row>
     <row r="190">
@@ -2512,10 +2512,10 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>0.002233788216832836</v>
+        <v>0.002209555287991798</v>
       </c>
       <c r="C190" t="n">
-        <v>0.002300626099857207</v>
+        <v>0.002462796178059725</v>
       </c>
     </row>
     <row r="191">
@@ -2523,10 +2523,10 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>0.002105214892723824</v>
+        <v>0.002191959925915584</v>
       </c>
       <c r="C191" t="n">
-        <v>0.002300626099857207</v>
+        <v>0.002462796178059725</v>
       </c>
     </row>
     <row r="192">
@@ -2534,10 +2534,10 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>0.002084587307713119</v>
+        <v>0.002121638870326258</v>
       </c>
       <c r="C192" t="n">
-        <v>0.002288044208005071</v>
+        <v>0.002431349345789443</v>
       </c>
     </row>
     <row r="193">
@@ -2545,10 +2545,10 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>0.002084587307713119</v>
+        <v>0.002050732140924637</v>
       </c>
       <c r="C193" t="n">
-        <v>0.002226672658292317</v>
+        <v>0.002411415821444678</v>
       </c>
     </row>
     <row r="194">
@@ -2556,10 +2556,10 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>0.002077843576485175</v>
+        <v>0.002026299158148671</v>
       </c>
       <c r="C194" t="n">
-        <v>0.002167226414848081</v>
+        <v>0.002411415821444678</v>
       </c>
     </row>
     <row r="195">
@@ -2567,10 +2567,10 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>0.002077843576485175</v>
+        <v>0.001995773971008738</v>
       </c>
       <c r="C195" t="n">
-        <v>0.002089568391780767</v>
+        <v>0.002392907639625884</v>
       </c>
     </row>
     <row r="196">
@@ -2578,10 +2578,10 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>0.002077843576485175</v>
+        <v>0.001986986292063403</v>
       </c>
       <c r="C196" t="n">
-        <v>0.002089568391780767</v>
+        <v>0.002378657909356249</v>
       </c>
     </row>
     <row r="197">
@@ -2589,10 +2589,10 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>0.002032033209354755</v>
+        <v>0.001982720746568073</v>
       </c>
       <c r="C197" t="n">
-        <v>0.002022121388777632</v>
+        <v>0.00234612775871571</v>
       </c>
     </row>
     <row r="198">
@@ -2600,10 +2600,10 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>0.002032033209354755</v>
+        <v>0.001982720746568073</v>
       </c>
       <c r="C198" t="n">
-        <v>0.002022121388777632</v>
+        <v>0.00234612775871571</v>
       </c>
     </row>
     <row r="199">
@@ -2611,10 +2611,10 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>0.00199019643335992</v>
+        <v>0.001981532587256143</v>
       </c>
       <c r="C199" t="n">
-        <v>0.002018836761120578</v>
+        <v>0.00234612775871571</v>
       </c>
     </row>
     <row r="200">
@@ -2622,10 +2622,10 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>0.001960636390853698</v>
+        <v>0.001974639932901239</v>
       </c>
       <c r="C200" t="n">
-        <v>0.001995753134636668</v>
+        <v>0.002341484932226634</v>
       </c>
     </row>
     <row r="201">
@@ -2633,10 +2633,10 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>0.001931095821372788</v>
+        <v>0.001964433406208879</v>
       </c>
       <c r="C201" t="n">
-        <v>0.001971381533321776</v>
+        <v>0.002341484932226634</v>
       </c>
     </row>
     <row r="202">
@@ -2644,10 +2644,10 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>0.001870537710814002</v>
+        <v>0.001936180782222836</v>
       </c>
       <c r="C202" t="n">
-        <v>0.001930794080626776</v>
+        <v>0.002250235163910151</v>
       </c>
     </row>
     <row r="203">
@@ -2655,10 +2655,10 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>0.001870537710814002</v>
+        <v>0.00186643931027709</v>
       </c>
       <c r="C203" t="n">
-        <v>0.0019226402993454</v>
+        <v>0.002246502792347751</v>
       </c>
     </row>
     <row r="204">
@@ -2666,10 +2666,10 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>0.001860082559293735</v>
+        <v>0.001853068077918427</v>
       </c>
       <c r="C204" t="n">
-        <v>0.001906458591859518</v>
+        <v>0.002207631795566664</v>
       </c>
     </row>
     <row r="205">
@@ -2677,10 +2677,10 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
-        <v>0.001855794323696088</v>
+        <v>0.001834068239360157</v>
       </c>
       <c r="C205" t="n">
-        <v>0.001878124234683907</v>
+        <v>0.002200953739074901</v>
       </c>
     </row>
     <row r="206">
@@ -2688,10 +2688,10 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>0.001851924208180635</v>
+        <v>0.001834068239360157</v>
       </c>
       <c r="C206" t="n">
-        <v>0.001835769166892141</v>
+        <v>0.002198063789573278</v>
       </c>
     </row>
     <row r="207">
@@ -2699,10 +2699,10 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>0.001851924208180635</v>
+        <v>0.001771216017314777</v>
       </c>
       <c r="C207" t="n">
-        <v>0.001782748865530024</v>
+        <v>0.002165250506161467</v>
       </c>
     </row>
     <row r="208">
@@ -2710,10 +2710,10 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>0.00183406042588984</v>
+        <v>0.001764518114074468</v>
       </c>
       <c r="C208" t="n">
-        <v>0.001782748865530024</v>
+        <v>0.002125905629121419</v>
       </c>
     </row>
     <row r="209">
@@ -2721,10 +2721,10 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>0.00182843016785095</v>
+        <v>0.001764518114074468</v>
       </c>
       <c r="C209" t="n">
-        <v>0.001749189946664058</v>
+        <v>0.002110836946035695</v>
       </c>
     </row>
     <row r="210">
@@ -2732,10 +2732,10 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>0.001786919757375225</v>
+        <v>0.001731427868693187</v>
       </c>
       <c r="C210" t="n">
-        <v>0.001747240541129961</v>
+        <v>0.001885976029117871</v>
       </c>
     </row>
     <row r="211">
@@ -2743,10 +2743,10 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>0.001702219722846877</v>
+        <v>0.001643498541640937</v>
       </c>
       <c r="C211" t="n">
-        <v>0.001551779390016937</v>
+        <v>0.001885976029117871</v>
       </c>
     </row>
     <row r="212">
@@ -2754,10 +2754,10 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>0.001685327053098624</v>
+        <v>0.001584989900555008</v>
       </c>
       <c r="C212" t="n">
-        <v>0.001527536078261349</v>
+        <v>0.001881384876853706</v>
       </c>
     </row>
     <row r="213">
@@ -2765,10 +2765,10 @@
         <v>211</v>
       </c>
       <c r="B213" t="n">
-        <v>0.001682271644012232</v>
+        <v>0.001470225282081323</v>
       </c>
       <c r="C213" t="n">
-        <v>0.00151574882454396</v>
+        <v>0.001851090760412635</v>
       </c>
     </row>
     <row r="214">
@@ -2776,10 +2776,10 @@
         <v>212</v>
       </c>
       <c r="B214" t="n">
-        <v>0.001682271644012232</v>
+        <v>0.00144145767804183</v>
       </c>
       <c r="C214" t="n">
-        <v>0.001497336507002566</v>
+        <v>0.001851090760412635</v>
       </c>
     </row>
     <row r="215">
@@ -2787,10 +2787,10 @@
         <v>213</v>
       </c>
       <c r="B215" t="n">
-        <v>0.001649169276915602</v>
+        <v>0.00142049408024758</v>
       </c>
       <c r="C215" t="n">
-        <v>0.001403581033269524</v>
+        <v>0.001851090760412635</v>
       </c>
     </row>
     <row r="216">
@@ -2798,10 +2798,10 @@
         <v>214</v>
       </c>
       <c r="B216" t="n">
-        <v>0.001649169276915602</v>
+        <v>0.001413010530326217</v>
       </c>
       <c r="C216" t="n">
-        <v>0.001322210809133282</v>
+        <v>0.001818303825376524</v>
       </c>
     </row>
     <row r="217">
@@ -2809,10 +2809,10 @@
         <v>215</v>
       </c>
       <c r="B217" t="n">
-        <v>0.001649169276915602</v>
+        <v>0.001402211601608014</v>
       </c>
       <c r="C217" t="n">
-        <v>0.001321623711623398</v>
+        <v>0.001708481685312555</v>
       </c>
     </row>
     <row r="218">
@@ -2820,10 +2820,10 @@
         <v>216</v>
       </c>
       <c r="B218" t="n">
-        <v>0.001622799922136583</v>
+        <v>0.00137955289048051</v>
       </c>
       <c r="C218" t="n">
-        <v>0.001304681676971552</v>
+        <v>0.001702178962127482</v>
       </c>
     </row>
     <row r="219">
@@ -2831,10 +2831,10 @@
         <v>217</v>
       </c>
       <c r="B219" t="n">
-        <v>0.001584322087510266</v>
+        <v>0.00137955289048051</v>
       </c>
       <c r="C219" t="n">
-        <v>0.001304681676971552</v>
+        <v>0.001647721490099572</v>
       </c>
     </row>
     <row r="220">
@@ -2842,10 +2842,10 @@
         <v>218</v>
       </c>
       <c r="B220" t="n">
-        <v>0.001583244424535239</v>
+        <v>0.001341983953298935</v>
       </c>
       <c r="C220" t="n">
-        <v>0.001275562635908855</v>
+        <v>0.001607804963280499</v>
       </c>
     </row>
     <row r="221">
@@ -2853,10 +2853,10 @@
         <v>219</v>
       </c>
       <c r="B221" t="n">
-        <v>0.001516002088418676</v>
+        <v>0.001341859510089903</v>
       </c>
       <c r="C221" t="n">
-        <v>0.00126529638112685</v>
+        <v>0.001596360004259704</v>
       </c>
     </row>
     <row r="222">
@@ -2864,10 +2864,10 @@
         <v>220</v>
       </c>
       <c r="B222" t="n">
-        <v>0.001516002088418676</v>
+        <v>0.001341859510089903</v>
       </c>
       <c r="C222" t="n">
-        <v>0.001252906380909502</v>
+        <v>0.001592798489942602</v>
       </c>
     </row>
     <row r="223">
@@ -2875,10 +2875,10 @@
         <v>221</v>
       </c>
       <c r="B223" t="n">
-        <v>0.001506645728036543</v>
+        <v>0.001269677604682341</v>
       </c>
       <c r="C223" t="n">
-        <v>0.001241712820466102</v>
+        <v>0.001572388986302904</v>
       </c>
     </row>
     <row r="224">
@@ -2886,10 +2886,10 @@
         <v>222</v>
       </c>
       <c r="B224" t="n">
-        <v>0.001458631194365482</v>
+        <v>0.001240051168347343</v>
       </c>
       <c r="C224" t="n">
-        <v>0.001220663629578571</v>
+        <v>0.001446857453868788</v>
       </c>
     </row>
     <row r="225">
@@ -2897,10 +2897,10 @@
         <v>223</v>
       </c>
       <c r="B225" t="n">
-        <v>0.001452443508087051</v>
+        <v>0.001207574929040235</v>
       </c>
       <c r="C225" t="n">
-        <v>0.001220663629578571</v>
+        <v>0.001412819987344111</v>
       </c>
     </row>
     <row r="226">
@@ -2908,10 +2908,10 @@
         <v>224</v>
       </c>
       <c r="B226" t="n">
-        <v>0.001429271222271293</v>
+        <v>0.001196436543210057</v>
       </c>
       <c r="C226" t="n">
-        <v>0.001214194925786211</v>
+        <v>0.001409206818025365</v>
       </c>
     </row>
     <row r="227">
@@ -2919,10 +2919,10 @@
         <v>225</v>
       </c>
       <c r="B227" t="n">
-        <v>0.001421963499095724</v>
+        <v>0.001196436543210057</v>
       </c>
       <c r="C227" t="n">
-        <v>0.001205119600023275</v>
+        <v>0.001394946835884161</v>
       </c>
     </row>
     <row r="228">
@@ -2930,10 +2930,10 @@
         <v>226</v>
       </c>
       <c r="B228" t="n">
-        <v>0.001353505502695202</v>
+        <v>0.0011541879501821</v>
       </c>
       <c r="C228" t="n">
-        <v>0.001201012512098664</v>
+        <v>0.001372381613627405</v>
       </c>
     </row>
     <row r="229">
@@ -2941,10 +2941,10 @@
         <v>227</v>
       </c>
       <c r="B229" t="n">
-        <v>0.001273816846317685</v>
+        <v>0.001129252374338626</v>
       </c>
       <c r="C229" t="n">
-        <v>0.001195623369821198</v>
+        <v>0.0013378625215291</v>
       </c>
     </row>
     <row r="230">
@@ -2952,10 +2952,10 @@
         <v>228</v>
       </c>
       <c r="B230" t="n">
-        <v>0.001273816846317685</v>
+        <v>0.001127130376136301</v>
       </c>
       <c r="C230" t="n">
-        <v>0.001181885539106332</v>
+        <v>0.001329667933649062</v>
       </c>
     </row>
     <row r="231">
@@ -2963,10 +2963,10 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>0.001212591968257399</v>
+        <v>0.001011447802106824</v>
       </c>
       <c r="C231" t="n">
-        <v>0.001181885539106332</v>
+        <v>0.00125551507066009</v>
       </c>
     </row>
     <row r="232">
@@ -2974,10 +2974,10 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>0.001182351487835864</v>
+        <v>0.000980893119604931</v>
       </c>
       <c r="C232" t="n">
-        <v>0.001126051651388659</v>
+        <v>0.001240733493107933</v>
       </c>
     </row>
     <row r="233">
@@ -2985,10 +2985,10 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>0.00114798674808325</v>
+        <v>0.0009734417015154613</v>
       </c>
       <c r="C233" t="n">
-        <v>0.001098681317595259</v>
+        <v>0.001191173805203474</v>
       </c>
     </row>
     <row r="234">
@@ -2996,10 +2996,10 @@
         <v>232</v>
       </c>
       <c r="B234" t="n">
-        <v>0.001082548353744386</v>
+        <v>0.0009645852201644666</v>
       </c>
       <c r="C234" t="n">
-        <v>0.001098681317595259</v>
+        <v>0.001191173805203474</v>
       </c>
     </row>
     <row r="235">
@@ -3007,10 +3007,10 @@
         <v>233</v>
       </c>
       <c r="B235" t="n">
-        <v>0.001044021014041921</v>
+        <v>0.0009545666286000904</v>
       </c>
       <c r="C235" t="n">
-        <v>0.00107080271999072</v>
+        <v>0.00118326433037997</v>
       </c>
     </row>
     <row r="236">
@@ -3018,10 +3018,10 @@
         <v>234</v>
       </c>
       <c r="B236" t="n">
-        <v>0.001044021014041921</v>
+        <v>0.0009408984146401356</v>
       </c>
       <c r="C236" t="n">
-        <v>0.001056151141733776</v>
+        <v>0.001162056781921724</v>
       </c>
     </row>
     <row r="237">
@@ -3029,10 +3029,10 @@
         <v>235</v>
       </c>
       <c r="B237" t="n">
-        <v>0.001044021014041921</v>
+        <v>0.0009340717028402562</v>
       </c>
       <c r="C237" t="n">
-        <v>0.001054424279157914</v>
+        <v>0.001147643838650306</v>
       </c>
     </row>
     <row r="238">
@@ -3040,10 +3040,10 @@
         <v>236</v>
       </c>
       <c r="B238" t="n">
-        <v>0.001028313152983812</v>
+        <v>0.0009319494027583053</v>
       </c>
       <c r="C238" t="n">
-        <v>0.001054424279157914</v>
+        <v>0.001082597244465764</v>
       </c>
     </row>
     <row r="239">
@@ -3051,10 +3051,10 @@
         <v>237</v>
       </c>
       <c r="B239" t="n">
-        <v>0.001028063643648024</v>
+        <v>0.0008693662259030567</v>
       </c>
       <c r="C239" t="n">
-        <v>0.001044186190767725</v>
+        <v>0.001082597244465764</v>
       </c>
     </row>
     <row r="240">
@@ -3062,10 +3062,10 @@
         <v>238</v>
       </c>
       <c r="B240" t="n">
-        <v>0.001017697492462218</v>
+        <v>0.0008344724666296022</v>
       </c>
       <c r="C240" t="n">
-        <v>0.001044186190767725</v>
+        <v>0.001072520553059968</v>
       </c>
     </row>
     <row r="241">
@@ -3073,10 +3073,10 @@
         <v>239</v>
       </c>
       <c r="B241" t="n">
-        <v>0.001014952491322558</v>
+        <v>0.0008265739218468536</v>
       </c>
       <c r="C241" t="n">
-        <v>0.00103793615645918</v>
+        <v>0.001067378171265917</v>
       </c>
     </row>
     <row r="242">
@@ -3084,10 +3084,10 @@
         <v>240</v>
       </c>
       <c r="B242" t="n">
-        <v>0.0009966553681463701</v>
+        <v>0.000811564315384714</v>
       </c>
       <c r="C242" t="n">
-        <v>0.001017705990783622</v>
+        <v>0.001060318429148508</v>
       </c>
     </row>
     <row r="243">
@@ -3095,10 +3095,10 @@
         <v>241</v>
       </c>
       <c r="B243" t="n">
-        <v>0.0009879506652530744</v>
+        <v>0.000811564315384714</v>
       </c>
       <c r="C243" t="n">
-        <v>0.001017705990783622</v>
+        <v>0.001059182687142209</v>
       </c>
     </row>
     <row r="244">
@@ -3106,10 +3106,10 @@
         <v>242</v>
       </c>
       <c r="B244" t="n">
-        <v>0.0009837098325887006</v>
+        <v>0.0007970336924170361</v>
       </c>
       <c r="C244" t="n">
-        <v>0.000983976378988454</v>
+        <v>0.001055939665590399</v>
       </c>
     </row>
     <row r="245">
@@ -3117,10 +3117,10 @@
         <v>243</v>
       </c>
       <c r="B245" t="n">
-        <v>0.0009646185226478281</v>
+        <v>0.0007811485566188283</v>
       </c>
       <c r="C245" t="n">
-        <v>0.0009826538690900222</v>
+        <v>0.001051562764250449</v>
       </c>
     </row>
     <row r="246">
@@ -3128,10 +3128,10 @@
         <v>244</v>
       </c>
       <c r="B246" t="n">
-        <v>0.0009289350536769165</v>
+        <v>0.0007516386204196568</v>
       </c>
       <c r="C246" t="n">
-        <v>0.0009826538690900222</v>
+        <v>0.001043373146826077</v>
       </c>
     </row>
     <row r="247">
@@ -3139,10 +3139,10 @@
         <v>245</v>
       </c>
       <c r="B247" t="n">
-        <v>0.0008868658778998223</v>
+        <v>0.000751221873242338</v>
       </c>
       <c r="C247" t="n">
-        <v>0.000979226546061281</v>
+        <v>0.001043373146826077</v>
       </c>
     </row>
     <row r="248">
@@ -3150,10 +3150,10 @@
         <v>246</v>
       </c>
       <c r="B248" t="n">
-        <v>0.0008400660694714359</v>
+        <v>0.000751221873242338</v>
       </c>
       <c r="C248" t="n">
-        <v>0.0009575525879454641</v>
+        <v>0.001000237541051128</v>
       </c>
     </row>
     <row r="249">
@@ -3161,10 +3161,10 @@
         <v>247</v>
       </c>
       <c r="B249" t="n">
-        <v>0.0008400660694714359</v>
+        <v>0.0007222075275066426</v>
       </c>
       <c r="C249" t="n">
-        <v>0.0009498731476667507</v>
+        <v>0.0009781116138727665</v>
       </c>
     </row>
     <row r="250">
@@ -3172,10 +3172,10 @@
         <v>248</v>
       </c>
       <c r="B250" t="n">
-        <v>0.0008346665410923361</v>
+        <v>0.0007083123516848184</v>
       </c>
       <c r="C250" t="n">
-        <v>0.0009214316194035189</v>
+        <v>0.0009781116138727665</v>
       </c>
     </row>
     <row r="251">
@@ -3183,10 +3183,10 @@
         <v>249</v>
       </c>
       <c r="B251" t="n">
-        <v>0.0008117742515706327</v>
+        <v>0.0007083123516848184</v>
       </c>
       <c r="C251" t="n">
-        <v>0.0009187628847085647</v>
+        <v>0.0009507525323669006</v>
       </c>
     </row>
     <row r="252">
@@ -3194,10 +3194,10 @@
         <v>250</v>
       </c>
       <c r="B252" t="n">
-        <v>0.0007890451062668193</v>
+        <v>0.0006952011302803168</v>
       </c>
       <c r="C252" t="n">
-        <v>0.0009033352813686413</v>
+        <v>0.0009041312176073417</v>
       </c>
     </row>
     <row r="253">
@@ -3205,10 +3205,10 @@
         <v>251</v>
       </c>
       <c r="B253" t="n">
-        <v>0.0007748082016451087</v>
+        <v>0.0006936408365736055</v>
       </c>
       <c r="C253" t="n">
-        <v>0.0008746039659457621</v>
+        <v>0.0009041312176073417</v>
       </c>
     </row>
     <row r="254">
@@ -3216,10 +3216,10 @@
         <v>252</v>
       </c>
       <c r="B254" t="n">
-        <v>0.0007707294481350771</v>
+        <v>0.0006936408365736055</v>
       </c>
       <c r="C254" t="n">
-        <v>0.0008654312994253982</v>
+        <v>0.0009041312176073417</v>
       </c>
     </row>
     <row r="255">
@@ -3227,10 +3227,10 @@
         <v>253</v>
       </c>
       <c r="B255" t="n">
-        <v>0.0007559278033271802</v>
+        <v>0.0006698396773091265</v>
       </c>
       <c r="C255" t="n">
-        <v>0.0008475160448605265</v>
+        <v>0.0008936270675903168</v>
       </c>
     </row>
     <row r="256">
@@ -3238,10 +3238,10 @@
         <v>254</v>
       </c>
       <c r="B256" t="n">
-        <v>0.0007442033401210507</v>
+        <v>0.0006698396773091265</v>
       </c>
       <c r="C256" t="n">
-        <v>0.0008364153523875423</v>
+        <v>0.0008936270675903168</v>
       </c>
     </row>
     <row r="257">
@@ -3249,10 +3249,10 @@
         <v>255</v>
       </c>
       <c r="B257" t="n">
-        <v>0.0007442033401210507</v>
+        <v>0.0006628934695556522</v>
       </c>
       <c r="C257" t="n">
-        <v>0.0008364153523875423</v>
+        <v>0.0008787128298586165</v>
       </c>
     </row>
     <row r="258">
@@ -3260,10 +3260,10 @@
         <v>256</v>
       </c>
       <c r="B258" t="n">
-        <v>0.0007161839143497112</v>
+        <v>0.0006628934695556522</v>
       </c>
       <c r="C258" t="n">
-        <v>0.0008169118409060691</v>
+        <v>0.0008240561089825829</v>
       </c>
     </row>
     <row r="259">
@@ -3271,10 +3271,10 @@
         <v>257</v>
       </c>
       <c r="B259" t="n">
-        <v>0.0007115512622239704</v>
+        <v>0.0006374480894375477</v>
       </c>
       <c r="C259" t="n">
-        <v>0.0008000606253672579</v>
+        <v>0.0008176741318205681</v>
       </c>
     </row>
     <row r="260">
@@ -3282,10 +3282,10 @@
         <v>258</v>
       </c>
       <c r="B260" t="n">
-        <v>0.0006810125708856614</v>
+        <v>0.0006374480894375477</v>
       </c>
       <c r="C260" t="n">
-        <v>0.0008000606253672579</v>
+        <v>0.0008115678928491493</v>
       </c>
     </row>
     <row r="261">
@@ -3293,10 +3293,10 @@
         <v>259</v>
       </c>
       <c r="B261" t="n">
-        <v>0.0006801871476732746</v>
+        <v>0.0006260813299789853</v>
       </c>
       <c r="C261" t="n">
-        <v>0.0008000606253672579</v>
+        <v>0.0007952787662621106</v>
       </c>
     </row>
     <row r="262">
@@ -3304,10 +3304,10 @@
         <v>260</v>
       </c>
       <c r="B262" t="n">
-        <v>0.0006590903249315817</v>
+        <v>0.0006103122619763967</v>
       </c>
       <c r="C262" t="n">
-        <v>0.0007905632288714025</v>
+        <v>0.0007776033863226397</v>
       </c>
     </row>
     <row r="263">
@@ -3315,10 +3315,10 @@
         <v>261</v>
       </c>
       <c r="B263" t="n">
-        <v>0.0006546995188380659</v>
+        <v>0.0005979376670734581</v>
       </c>
       <c r="C263" t="n">
-        <v>0.0007755122634944455</v>
+        <v>0.0007408518887708698</v>
       </c>
     </row>
     <row r="264">
@@ -3326,10 +3326,10 @@
         <v>262</v>
       </c>
       <c r="B264" t="n">
-        <v>0.0006334889442113442</v>
+        <v>0.0005960888985776194</v>
       </c>
       <c r="C264" t="n">
-        <v>0.0007373676248425559</v>
+        <v>0.0007237993075819911</v>
       </c>
     </row>
     <row r="265">
@@ -3337,10 +3337,10 @@
         <v>263</v>
       </c>
       <c r="B265" t="n">
-        <v>0.0006163059590398577</v>
+        <v>0.0005888334290139976</v>
       </c>
       <c r="C265" t="n">
-        <v>0.0007240222239714895</v>
+        <v>0.0007237993075819911</v>
       </c>
     </row>
     <row r="266">
@@ -3348,10 +3348,10 @@
         <v>264</v>
       </c>
       <c r="B266" t="n">
-        <v>0.0005973441972210581</v>
+        <v>0.0005808500602411901</v>
       </c>
       <c r="C266" t="n">
-        <v>0.0007099848569396877</v>
+        <v>0.0007216762430210786</v>
       </c>
     </row>
     <row r="267">
@@ -3359,10 +3359,10 @@
         <v>265</v>
       </c>
       <c r="B267" t="n">
-        <v>0.0005936044641471298</v>
+        <v>0.0005748548723938491</v>
       </c>
       <c r="C267" t="n">
-        <v>0.0006893455947836622</v>
+        <v>0.0007158903186626793</v>
       </c>
     </row>
     <row r="268">
@@ -3370,10 +3370,10 @@
         <v>266</v>
       </c>
       <c r="B268" t="n">
-        <v>0.0005916440044736542</v>
+        <v>0.00055424390829311</v>
       </c>
       <c r="C268" t="n">
-        <v>0.0006860039065159705</v>
+        <v>0.0006960775458201072</v>
       </c>
     </row>
     <row r="269">
@@ -3381,10 +3381,10 @@
         <v>267</v>
       </c>
       <c r="B269" t="n">
-        <v>0.0005916440044736542</v>
+        <v>0.0005366084671611401</v>
       </c>
       <c r="C269" t="n">
-        <v>0.0006688489199665861</v>
+        <v>0.0006925096547285496</v>
       </c>
     </row>
     <row r="270">
@@ -3392,10 +3392,10 @@
         <v>268</v>
       </c>
       <c r="B270" t="n">
-        <v>0.000575937979488228</v>
+        <v>0.0005243245807486406</v>
       </c>
       <c r="C270" t="n">
-        <v>0.0006582053644605222</v>
+        <v>0.0006792968462556335</v>
       </c>
     </row>
     <row r="271">
@@ -3403,10 +3403,10 @@
         <v>269</v>
       </c>
       <c r="B271" t="n">
-        <v>0.0005758470501279274</v>
+        <v>0.000523816583820989</v>
       </c>
       <c r="C271" t="n">
-        <v>0.0006340080513887083</v>
+        <v>0.0006666047782867943</v>
       </c>
     </row>
     <row r="272">
@@ -3414,10 +3414,10 @@
         <v>270</v>
       </c>
       <c r="B272" t="n">
-        <v>0.0005670918394980307</v>
+        <v>0.0005233281458757975</v>
       </c>
       <c r="C272" t="n">
-        <v>0.0006185523152776678</v>
+        <v>0.0006519371312116292</v>
       </c>
     </row>
     <row r="273">
@@ -3425,10 +3425,10 @@
         <v>271</v>
       </c>
       <c r="B273" t="n">
-        <v>0.0005588907643326535</v>
+        <v>0.0005106084784905287</v>
       </c>
       <c r="C273" t="n">
-        <v>0.0006095018610831143</v>
+        <v>0.0006519371312116292</v>
       </c>
     </row>
     <row r="274">
@@ -3436,10 +3436,10 @@
         <v>272</v>
       </c>
       <c r="B274" t="n">
-        <v>0.0005588907643326535</v>
+        <v>0.0005106084784905287</v>
       </c>
       <c r="C274" t="n">
-        <v>0.0006073598272130509</v>
+        <v>0.0006269488884128622</v>
       </c>
     </row>
     <row r="275">
@@ -3447,10 +3447,10 @@
         <v>273</v>
       </c>
       <c r="B275" t="n">
-        <v>0.0005564975105986542</v>
+        <v>0.0004866132688763821</v>
       </c>
       <c r="C275" t="n">
-        <v>0.0006031215686333149</v>
+        <v>0.000610432731815883</v>
       </c>
     </row>
     <row r="276">
@@ -3458,10 +3458,10 @@
         <v>274</v>
       </c>
       <c r="B276" t="n">
-        <v>0.0005401455029839679</v>
+        <v>0.0004786510393050246</v>
       </c>
       <c r="C276" t="n">
-        <v>0.0006031215686333149</v>
+        <v>0.0006037915909433144</v>
       </c>
     </row>
     <row r="277">
@@ -3469,10 +3469,10 @@
         <v>275</v>
       </c>
       <c r="B277" t="n">
-        <v>0.0005205848425142495</v>
+        <v>0.0004775234598849573</v>
       </c>
       <c r="C277" t="n">
-        <v>0.0006031215686333149</v>
+        <v>0.0005951553457846346</v>
       </c>
     </row>
     <row r="278">
@@ -3480,10 +3480,10 @@
         <v>276</v>
       </c>
       <c r="B278" t="n">
-        <v>0.0005169351187207777</v>
+        <v>0.0004720337590425113</v>
       </c>
       <c r="C278" t="n">
-        <v>0.0005883866398459985</v>
+        <v>0.0005741657184286735</v>
       </c>
     </row>
     <row r="279">
@@ -3491,10 +3491,10 @@
         <v>277</v>
       </c>
       <c r="B279" t="n">
-        <v>0.0005033838401774504</v>
+        <v>0.000461702054391901</v>
       </c>
       <c r="C279" t="n">
-        <v>0.0005790658080331711</v>
+        <v>0.0005648040363983809</v>
       </c>
     </row>
     <row r="280">
@@ -3502,10 +3502,10 @@
         <v>278</v>
       </c>
       <c r="B280" t="n">
-        <v>0.0005021395644890436</v>
+        <v>0.0004518028332592197</v>
       </c>
       <c r="C280" t="n">
-        <v>0.0005525791079239826</v>
+        <v>0.0005601891396797293</v>
       </c>
     </row>
     <row r="281">
@@ -3513,10 +3513,10 @@
         <v>279</v>
       </c>
       <c r="B281" t="n">
-        <v>0.000490280941650707</v>
+        <v>0.0004466189288874977</v>
       </c>
       <c r="C281" t="n">
-        <v>0.0005234370626320071</v>
+        <v>0.0005601891396797293</v>
       </c>
     </row>
     <row r="282">
@@ -3524,10 +3524,10 @@
         <v>280</v>
       </c>
       <c r="B282" t="n">
-        <v>0.0004791760295457808</v>
+        <v>0.0004385943467273353</v>
       </c>
       <c r="C282" t="n">
-        <v>0.0005198258707599597</v>
+        <v>0.0005419426037093806</v>
       </c>
     </row>
     <row r="283">
@@ -3535,10 +3535,10 @@
         <v>281</v>
       </c>
       <c r="B283" t="n">
-        <v>0.000472607738801282</v>
+        <v>0.0004312693087232984</v>
       </c>
       <c r="C283" t="n">
-        <v>0.0005129206937641309</v>
+        <v>0.0005238828912632211</v>
       </c>
     </row>
     <row r="284">
@@ -3546,10 +3546,10 @@
         <v>282</v>
       </c>
       <c r="B284" t="n">
-        <v>0.000465117977214738</v>
+        <v>0.000419790422937022</v>
       </c>
       <c r="C284" t="n">
-        <v>0.0005129206937641309</v>
+        <v>0.0005105216130055668</v>
       </c>
     </row>
     <row r="285">
@@ -3557,10 +3557,10 @@
         <v>283</v>
       </c>
       <c r="B285" t="n">
-        <v>0.000465117977214738</v>
+        <v>0.000413534353282994</v>
       </c>
       <c r="C285" t="n">
-        <v>0.0005129206937641309</v>
+        <v>0.0004998349991328687</v>
       </c>
     </row>
     <row r="286">
@@ -3568,10 +3568,10 @@
         <v>284</v>
       </c>
       <c r="B286" t="n">
-        <v>0.0004555104696820506</v>
+        <v>0.0004085512812248811</v>
       </c>
       <c r="C286" t="n">
-        <v>0.0005103509380810321</v>
+        <v>0.0004771649473138994</v>
       </c>
     </row>
     <row r="287">
@@ -3579,10 +3579,10 @@
         <v>285</v>
       </c>
       <c r="B287" t="n">
-        <v>0.0004555104696820506</v>
+        <v>0.0004042684168118411</v>
       </c>
       <c r="C287" t="n">
-        <v>0.0005103509380810321</v>
+        <v>0.0004694702046532619</v>
       </c>
     </row>
     <row r="288">
@@ -3590,10 +3590,10 @@
         <v>286</v>
       </c>
       <c r="B288" t="n">
-        <v>0.0004508307839611799</v>
+        <v>0.0003867297053112819</v>
       </c>
       <c r="C288" t="n">
-        <v>0.0005006549982629423</v>
+        <v>0.0004304115547428973</v>
       </c>
     </row>
     <row r="289">
@@ -3601,10 +3601,10 @@
         <v>287</v>
       </c>
       <c r="B289" t="n">
-        <v>0.0004508307839611799</v>
+        <v>0.0003718015184573868</v>
       </c>
       <c r="C289" t="n">
-        <v>0.000497381518117358</v>
+        <v>0.0004183516302740734</v>
       </c>
     </row>
     <row r="290">
@@ -3612,10 +3612,10 @@
         <v>288</v>
       </c>
       <c r="B290" t="n">
-        <v>0.0004349261839129205</v>
+        <v>0.0003627691568582785</v>
       </c>
       <c r="C290" t="n">
-        <v>0.0004650415213640624</v>
+        <v>0.00041412984463662</v>
       </c>
     </row>
     <row r="291">
@@ -3623,10 +3623,10 @@
         <v>289</v>
       </c>
       <c r="B291" t="n">
-        <v>0.0004247244862619888</v>
+        <v>0.000360654114648236</v>
       </c>
       <c r="C291" t="n">
-        <v>0.0004541918580002117</v>
+        <v>0.0004132787203246734</v>
       </c>
     </row>
     <row r="292">
@@ -3634,10 +3634,10 @@
         <v>290</v>
       </c>
       <c r="B292" t="n">
-        <v>0.0004236016193771975</v>
+        <v>0.0003600961019414282</v>
       </c>
       <c r="C292" t="n">
-        <v>0.0004498510515794101</v>
+        <v>0.0004130521098732462</v>
       </c>
     </row>
     <row r="293">
@@ -3645,10 +3645,10 @@
         <v>291</v>
       </c>
       <c r="B293" t="n">
-        <v>0.0004209397383853146</v>
+        <v>0.0003561516940870489</v>
       </c>
       <c r="C293" t="n">
-        <v>0.00043643290539052</v>
+        <v>0.0004130521098732462</v>
       </c>
     </row>
     <row r="294">
@@ -3656,10 +3656,10 @@
         <v>292</v>
       </c>
       <c r="B294" t="n">
-        <v>0.0004080183766574203</v>
+        <v>0.0003511512087688858</v>
       </c>
       <c r="C294" t="n">
-        <v>0.00043643290539052</v>
+        <v>0.0004044287734214831</v>
       </c>
     </row>
     <row r="295">
@@ -3667,10 +3667,10 @@
         <v>293</v>
       </c>
       <c r="B295" t="n">
-        <v>0.000394117841052684</v>
+        <v>0.000339809214175022</v>
       </c>
       <c r="C295" t="n">
-        <v>0.0004319396291649512</v>
+        <v>0.0004025144940100664</v>
       </c>
     </row>
     <row r="296">
@@ -3678,10 +3678,10 @@
         <v>294</v>
       </c>
       <c r="B296" t="n">
-        <v>0.0003824426926547016</v>
+        <v>0.0003371710583193556</v>
       </c>
       <c r="C296" t="n">
-        <v>0.0004290385640893659</v>
+        <v>0.0003874416093857363</v>
       </c>
     </row>
     <row r="297">
@@ -3689,10 +3689,10 @@
         <v>295</v>
       </c>
       <c r="B297" t="n">
-        <v>0.0003655767357080658</v>
+        <v>0.0003073722565912947</v>
       </c>
       <c r="C297" t="n">
-        <v>0.0004216575674090424</v>
+        <v>0.000383393493851873</v>
       </c>
     </row>
     <row r="298">
@@ -3700,10 +3700,10 @@
         <v>296</v>
       </c>
       <c r="B298" t="n">
-        <v>0.0003648827853367363</v>
+        <v>0.000306913430000636</v>
       </c>
       <c r="C298" t="n">
-        <v>0.000418793804011822</v>
+        <v>0.0003754191822575854</v>
       </c>
     </row>
     <row r="299">
@@ -3711,10 +3711,10 @@
         <v>297</v>
       </c>
       <c r="B299" t="n">
-        <v>0.0003618683487304863</v>
+        <v>0.0003007868369890574</v>
       </c>
       <c r="C299" t="n">
-        <v>0.0004092792285280107</v>
+        <v>0.0003731380449670371</v>
       </c>
     </row>
     <row r="300">
@@ -3722,10 +3722,10 @@
         <v>298</v>
       </c>
       <c r="B300" t="n">
-        <v>0.0003618683487304863</v>
+        <v>0.0002979482283130319</v>
       </c>
       <c r="C300" t="n">
-        <v>0.0004048903865154518</v>
+        <v>0.0003731380449670371</v>
       </c>
     </row>
     <row r="301">
@@ -3733,10 +3733,10 @@
         <v>299</v>
       </c>
       <c r="B301" t="n">
-        <v>0.0003612882716370351</v>
+        <v>0.0002885634068120011</v>
       </c>
       <c r="C301" t="n">
-        <v>0.0003987748671967584</v>
+        <v>0.0003694098912933094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>